<commit_message>
chore: update project files and dashboard pages
</commit_message>
<xml_diff>
--- a/backend/data/incubators.xlsx
+++ b/backend/data/incubators.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -430,787 +430,761 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="str">
-        <v>Edwards-Thomas Incubator</v>
+        <v>Baker, Salas and Nelson Incubator</v>
       </c>
       <c r="C2" t="str">
-        <v>Laura Reyes</v>
+        <v>Laura Taylor DVM</v>
       </c>
       <c r="D2" t="str">
-        <v>christianhernandez@hotmail.com</v>
+        <v>andrea11@lawrence.com</v>
       </c>
       <c r="E2" t="str">
-        <v>7934928252</v>
+        <v>+1-045-525-6450x772</v>
       </c>
       <c r="F2" t="str">
         <v>Blockchain</v>
       </c>
       <c r="G2" t="str">
-        <v>Afghanistan</v>
+        <v>Lesotho</v>
       </c>
       <c r="H2" t="str">
-        <v>Lisaview</v>
+        <v>Justinland</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="str">
-        <v>Baker, Salas and Nelson Incubator</v>
+        <v>Schaefer-Campbell Incubator</v>
       </c>
       <c r="C3" t="str">
-        <v>Laura Taylor DVM</v>
+        <v>Gene Dalton V</v>
       </c>
       <c r="D3" t="str">
-        <v>andrea11@lawrence.com</v>
+        <v>abell@gmail.com</v>
       </c>
       <c r="E3" t="str">
-        <v>+1-045-525-6450x772</v>
+        <v>522-600-9691x758</v>
       </c>
       <c r="F3" t="str">
-        <v>Blockchain</v>
+        <v>AI/ML</v>
       </c>
       <c r="G3" t="str">
-        <v>Lesotho</v>
+        <v>Serbia</v>
       </c>
       <c r="H3" t="str">
-        <v>Justinland</v>
+        <v>North Theresatown</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="str">
-        <v>Schaefer-Campbell Incubator</v>
+        <v>Stewart Group Incubator</v>
       </c>
       <c r="C4" t="str">
-        <v>Gene Dalton V</v>
+        <v>Courtney Downs</v>
       </c>
       <c r="D4" t="str">
-        <v>abell@gmail.com</v>
+        <v>roysmith@barber.biz</v>
       </c>
       <c r="E4" t="str">
-        <v>522-600-9691x758</v>
+        <v>291.776.4474x125</v>
       </c>
       <c r="F4" t="str">
-        <v>AI/ML</v>
+        <v>FinTech</v>
       </c>
       <c r="G4" t="str">
-        <v>Serbia</v>
+        <v>Burundi</v>
       </c>
       <c r="H4" t="str">
-        <v>North Theresatown</v>
+        <v>Brittanytown</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" t="str">
-        <v>Stewart Group Incubator</v>
+        <v>Fernandez-Diaz Incubator</v>
       </c>
       <c r="C5" t="str">
-        <v>Courtney Downs</v>
+        <v>David Cohen</v>
       </c>
       <c r="D5" t="str">
-        <v>roysmith@barber.biz</v>
+        <v>stephaniefoley@hotmail.com</v>
       </c>
       <c r="E5" t="str">
-        <v>291.776.4474x125</v>
+        <v>001-858-910-8567x3167</v>
       </c>
       <c r="F5" t="str">
-        <v>FinTech</v>
+        <v>AgriTech</v>
       </c>
       <c r="G5" t="str">
-        <v>Burundi</v>
+        <v>Korea</v>
       </c>
       <c r="H5" t="str">
-        <v>Brittanytown</v>
+        <v>East Stephen</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="str">
-        <v>Fernandez-Diaz Incubator</v>
+        <v>Ortega PLC Incubator</v>
       </c>
       <c r="C6" t="str">
-        <v>David Cohen</v>
+        <v>Allison Campbell</v>
       </c>
       <c r="D6" t="str">
-        <v>stephaniefoley@hotmail.com</v>
+        <v>cassidy84@hotmail.com</v>
       </c>
       <c r="E6" t="str">
-        <v>001-858-910-8567x3167</v>
+        <v>+1-369-183-5529</v>
       </c>
       <c r="F6" t="str">
-        <v>AgriTech</v>
+        <v>Cybersecurity</v>
       </c>
       <c r="G6" t="str">
-        <v>Korea</v>
+        <v>Azerbaijan</v>
       </c>
       <c r="H6" t="str">
-        <v>East Stephen</v>
+        <v>Davisshire</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" t="str">
-        <v>Ortega PLC Incubator</v>
+        <v>Young-Long Incubator</v>
       </c>
       <c r="C7" t="str">
-        <v>Allison Campbell</v>
+        <v>Bryan Salinas</v>
       </c>
       <c r="D7" t="str">
-        <v>cassidy84@hotmail.com</v>
+        <v>deannamason@acosta.com</v>
       </c>
       <c r="E7" t="str">
-        <v>+1-369-183-5529</v>
+        <v>907-601-2755</v>
       </c>
       <c r="F7" t="str">
-        <v>Cybersecurity</v>
+        <v>Biotech</v>
       </c>
       <c r="G7" t="str">
-        <v>Azerbaijan</v>
+        <v>Qatar</v>
       </c>
       <c r="H7" t="str">
-        <v>Davisshire</v>
+        <v>Kristenchester</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" t="str">
-        <v>Young-Long Incubator</v>
+        <v>Trujillo Ltd Incubator</v>
       </c>
       <c r="C8" t="str">
-        <v>Bryan Salinas</v>
+        <v>Joshua Serrano</v>
       </c>
       <c r="D8" t="str">
-        <v>deannamason@acosta.com</v>
+        <v>grayrobert@gmail.com</v>
       </c>
       <c r="E8" t="str">
-        <v>907-601-2755</v>
+        <v>4458470430</v>
       </c>
       <c r="F8" t="str">
-        <v>Biotech</v>
+        <v>Blockchain</v>
       </c>
       <c r="G8" t="str">
-        <v>Qatar</v>
+        <v>Sao Tome and Principe</v>
       </c>
       <c r="H8" t="str">
-        <v>Kristenchester</v>
+        <v>Kellyfort</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" t="str">
-        <v>Trujillo Ltd Incubator</v>
+        <v>Kennedy Inc Incubator</v>
       </c>
       <c r="C9" t="str">
-        <v>Joshua Serrano</v>
+        <v>Sean Wood</v>
       </c>
       <c r="D9" t="str">
-        <v>grayrobert@gmail.com</v>
+        <v>irodriguez@krueger.com</v>
       </c>
       <c r="E9" t="str">
-        <v>4458470430</v>
+        <v>282.841.0371x484</v>
       </c>
       <c r="F9" t="str">
         <v>Blockchain</v>
       </c>
       <c r="G9" t="str">
-        <v>Sao Tome and Principe</v>
+        <v>Belarus</v>
       </c>
       <c r="H9" t="str">
-        <v>Kellyfort</v>
+        <v>East Martin</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" t="str">
-        <v>Kennedy Inc Incubator</v>
+        <v>Vaughn, Davis and Robinson Incubator</v>
       </c>
       <c r="C10" t="str">
-        <v>Sean Wood</v>
+        <v>Albert Colon</v>
       </c>
       <c r="D10" t="str">
-        <v>irodriguez@krueger.com</v>
+        <v>juanguzman@yahoo.com</v>
       </c>
       <c r="E10" t="str">
-        <v>282.841.0371x484</v>
+        <v>057.692.9204x97248</v>
       </c>
       <c r="F10" t="str">
-        <v>Blockchain</v>
+        <v>FinTech</v>
       </c>
       <c r="G10" t="str">
-        <v>Belarus</v>
+        <v>Togo</v>
       </c>
       <c r="H10" t="str">
-        <v>East Martin</v>
+        <v>Carrollburgh</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" t="str">
-        <v>Vaughn, Davis and Robinson Incubator</v>
+        <v>Adams Inc Incubator</v>
       </c>
       <c r="C11" t="str">
-        <v>Albert Colon</v>
+        <v>Kenneth Houston</v>
       </c>
       <c r="D11" t="str">
-        <v>juanguzman@yahoo.com</v>
+        <v>john38@gmail.com</v>
       </c>
       <c r="E11" t="str">
-        <v>057.692.9204x97248</v>
+        <v>001-157-142-5360x4951</v>
       </c>
       <c r="F11" t="str">
-        <v>FinTech</v>
+        <v>HealthTech</v>
       </c>
       <c r="G11" t="str">
-        <v>Togo</v>
+        <v>Senegal</v>
       </c>
       <c r="H11" t="str">
-        <v>Carrollburgh</v>
+        <v>East Maryhaven</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" t="str">
-        <v>Adams Inc Incubator</v>
+        <v>Weaver LLC Incubator</v>
       </c>
       <c r="C12" t="str">
-        <v>Kenneth Houston</v>
+        <v>Robin Gonzales</v>
       </c>
       <c r="D12" t="str">
-        <v>john38@gmail.com</v>
+        <v>millerlinda@gmail.com</v>
       </c>
       <c r="E12" t="str">
-        <v>001-157-142-5360x4951</v>
+        <v>001-846-397-7006x1003</v>
       </c>
       <c r="F12" t="str">
-        <v>HealthTech</v>
+        <v>FinTech</v>
       </c>
       <c r="G12" t="str">
-        <v>Senegal</v>
+        <v>Tajikistan</v>
       </c>
       <c r="H12" t="str">
-        <v>East Maryhaven</v>
+        <v>West Ellen</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" t="str">
-        <v>Weaver LLC Incubator</v>
+        <v>Adams, Monroe and Bell Incubator</v>
       </c>
       <c r="C13" t="str">
-        <v>Robin Gonzales</v>
+        <v>Jeffrey Maynard</v>
       </c>
       <c r="D13" t="str">
-        <v>millerlinda@gmail.com</v>
+        <v>rebeccaperry@hotmail.com</v>
       </c>
       <c r="E13" t="str">
-        <v>001-846-397-7006x1003</v>
+        <v>364.945.1421</v>
       </c>
       <c r="F13" t="str">
-        <v>FinTech</v>
+        <v>Biotech</v>
       </c>
       <c r="G13" t="str">
-        <v>Tajikistan</v>
+        <v>Faroe Islands</v>
       </c>
       <c r="H13" t="str">
-        <v>West Ellen</v>
+        <v>East Cathybury</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" t="str">
-        <v>Adams, Monroe and Bell Incubator</v>
+        <v>Bates, Haas and Williams Incubator</v>
       </c>
       <c r="C14" t="str">
-        <v>Jeffrey Maynard</v>
+        <v>Brian Washington</v>
       </c>
       <c r="D14" t="str">
-        <v>rebeccaperry@hotmail.com</v>
+        <v>normafarmer@fuller.com</v>
       </c>
       <c r="E14" t="str">
-        <v>364.945.1421</v>
+        <v>001-053-359-0570x9871</v>
       </c>
       <c r="F14" t="str">
-        <v>Biotech</v>
+        <v>HealthTech</v>
       </c>
       <c r="G14" t="str">
-        <v>Faroe Islands</v>
+        <v>Mozambique</v>
       </c>
       <c r="H14" t="str">
-        <v>East Cathybury</v>
+        <v>Anthonyton</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" t="str">
-        <v>Bates, Haas and Williams Incubator</v>
+        <v>Phillips LLC Incubator</v>
       </c>
       <c r="C15" t="str">
-        <v>Brian Washington</v>
+        <v>Brandon Wallace</v>
       </c>
       <c r="D15" t="str">
-        <v>normafarmer@fuller.com</v>
+        <v>amymanning@lewis-henry.com</v>
       </c>
       <c r="E15" t="str">
-        <v>001-053-359-0570x9871</v>
+        <v>367-518-8179x871</v>
       </c>
       <c r="F15" t="str">
-        <v>HealthTech</v>
+        <v>Blockchain</v>
       </c>
       <c r="G15" t="str">
-        <v>Mozambique</v>
+        <v>Andorra</v>
       </c>
       <c r="H15" t="str">
-        <v>Anthonyton</v>
+        <v>North Josephburgh</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" t="str">
-        <v>Phillips LLC Incubator</v>
+        <v>Alvarez, Thompson and Taylor Incubator</v>
       </c>
       <c r="C16" t="str">
-        <v>Brandon Wallace</v>
+        <v>Angelica Gamble</v>
       </c>
       <c r="D16" t="str">
-        <v>amymanning@lewis-henry.com</v>
+        <v>zarnold@hotmail.com</v>
       </c>
       <c r="E16" t="str">
-        <v>367-518-8179x871</v>
+        <v>625.796.1725x68758</v>
       </c>
       <c r="F16" t="str">
-        <v>Blockchain</v>
+        <v>AI/ML</v>
       </c>
       <c r="G16" t="str">
-        <v>Andorra</v>
+        <v>Norway</v>
       </c>
       <c r="H16" t="str">
-        <v>North Josephburgh</v>
+        <v>South Shane</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" t="str">
-        <v>Alvarez, Thompson and Taylor Incubator</v>
+        <v>Hall-Page Incubator</v>
       </c>
       <c r="C17" t="str">
-        <v>Angelica Gamble</v>
+        <v>Aaron Brown</v>
       </c>
       <c r="D17" t="str">
-        <v>zarnold@hotmail.com</v>
+        <v>gkirby@hotmail.com</v>
       </c>
       <c r="E17" t="str">
-        <v>625.796.1725x68758</v>
+        <v>001-542-949-4976x95178</v>
       </c>
       <c r="F17" t="str">
-        <v>AI/ML</v>
+        <v>Clean Energy</v>
       </c>
       <c r="G17" t="str">
-        <v>Norway</v>
+        <v>Uganda</v>
       </c>
       <c r="H17" t="str">
-        <v>South Shane</v>
+        <v>Shorthaven</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" t="str">
-        <v>Hall-Page Incubator</v>
+        <v>Deleon-Holden Incubator</v>
       </c>
       <c r="C18" t="str">
-        <v>Aaron Brown</v>
+        <v>Phillip Hull</v>
       </c>
       <c r="D18" t="str">
-        <v>gkirby@hotmail.com</v>
+        <v>msmith@swanson-andrews.com</v>
       </c>
       <c r="E18" t="str">
-        <v>001-542-949-4976x95178</v>
+        <v>001-236-186-3545x70205</v>
       </c>
       <c r="F18" t="str">
-        <v>Clean Energy</v>
+        <v>Blockchain</v>
       </c>
       <c r="G18" t="str">
-        <v>Uganda</v>
+        <v>Equatorial Guinea</v>
       </c>
       <c r="H18" t="str">
-        <v>Shorthaven</v>
+        <v>Rachelfurt</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" t="str">
-        <v>Deleon-Holden Incubator</v>
+        <v>Merritt, Anderson and Cross Incubator</v>
       </c>
       <c r="C19" t="str">
-        <v>Phillip Hull</v>
+        <v>Brent Thomas</v>
       </c>
       <c r="D19" t="str">
-        <v>msmith@swanson-andrews.com</v>
+        <v>donovanbailey@smith-erickson.com</v>
       </c>
       <c r="E19" t="str">
-        <v>001-236-186-3545x70205</v>
+        <v>(044)565-4201</v>
       </c>
       <c r="F19" t="str">
-        <v>Blockchain</v>
+        <v>AI/ML</v>
       </c>
       <c r="G19" t="str">
-        <v>Equatorial Guinea</v>
+        <v>Myanmar</v>
       </c>
       <c r="H19" t="str">
-        <v>Rachelfurt</v>
+        <v>West Keith</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" t="str">
-        <v>Merritt, Anderson and Cross Incubator</v>
+        <v>Stone-Salazar Incubator</v>
       </c>
       <c r="C20" t="str">
-        <v>Brent Thomas</v>
+        <v>Edward Hunter</v>
       </c>
       <c r="D20" t="str">
-        <v>donovanbailey@smith-erickson.com</v>
+        <v>andrea60@gmail.com</v>
       </c>
       <c r="E20" t="str">
-        <v>(044)565-4201</v>
+        <v>211.655.2758x6849</v>
       </c>
       <c r="F20" t="str">
-        <v>AI/ML</v>
+        <v>EdTech</v>
       </c>
       <c r="G20" t="str">
-        <v>Myanmar</v>
+        <v>Iran</v>
       </c>
       <c r="H20" t="str">
-        <v>West Keith</v>
+        <v>Weavertown</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21" t="str">
-        <v>Stone-Salazar Incubator</v>
+        <v>Kaufman PLC Incubator</v>
       </c>
       <c r="C21" t="str">
-        <v>Edward Hunter</v>
+        <v>Tasha Hanson</v>
       </c>
       <c r="D21" t="str">
-        <v>andrea60@gmail.com</v>
+        <v>anitamorrison@hotmail.com</v>
       </c>
       <c r="E21" t="str">
-        <v>211.655.2758x6849</v>
+        <v>2522613276</v>
       </c>
       <c r="F21" t="str">
-        <v>EdTech</v>
+        <v>Blockchain</v>
       </c>
       <c r="G21" t="str">
-        <v>Iran</v>
+        <v>Algeria</v>
       </c>
       <c r="H21" t="str">
-        <v>Weavertown</v>
+        <v>Hensleychester</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" t="str">
-        <v>Kaufman PLC Incubator</v>
+        <v>Bruce-James Incubator</v>
       </c>
       <c r="C22" t="str">
-        <v>Tasha Hanson</v>
+        <v>Suzanne Matthews</v>
       </c>
       <c r="D22" t="str">
-        <v>anitamorrison@hotmail.com</v>
+        <v>hchandler@gmail.com</v>
       </c>
       <c r="E22" t="str">
-        <v>2522613276</v>
+        <v>+1-010-437-9859x119</v>
       </c>
       <c r="F22" t="str">
-        <v>Blockchain</v>
+        <v>HealthTech</v>
       </c>
       <c r="G22" t="str">
-        <v>Algeria</v>
+        <v>Aruba</v>
       </c>
       <c r="H22" t="str">
-        <v>Hensleychester</v>
+        <v>Welchchester</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" t="str">
-        <v>Bruce-James Incubator</v>
+        <v>Brown, Miller and Taylor Incubator</v>
       </c>
       <c r="C23" t="str">
-        <v>Suzanne Matthews</v>
+        <v>Martin Vazquez</v>
       </c>
       <c r="D23" t="str">
-        <v>hchandler@gmail.com</v>
+        <v>kwilson@hill-munoz.com</v>
       </c>
       <c r="E23" t="str">
-        <v>+1-010-437-9859x119</v>
+        <v>(397)708-5273x153</v>
       </c>
       <c r="F23" t="str">
         <v>HealthTech</v>
       </c>
       <c r="G23" t="str">
-        <v>Aruba</v>
+        <v>Fiji</v>
       </c>
       <c r="H23" t="str">
-        <v>Welchchester</v>
+        <v>Blackburnbury</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" t="str">
-        <v>Brown, Miller and Taylor Incubator</v>
+        <v>Smith Ltd Incubator</v>
       </c>
       <c r="C24" t="str">
-        <v>Martin Vazquez</v>
+        <v>Brooke Allen</v>
       </c>
       <c r="D24" t="str">
-        <v>kwilson@hill-munoz.com</v>
+        <v>margaret59@hotmail.com</v>
       </c>
       <c r="E24" t="str">
-        <v>(397)708-5273x153</v>
+        <v>279.800.0891</v>
       </c>
       <c r="F24" t="str">
-        <v>HealthTech</v>
+        <v>Clean Energy</v>
       </c>
       <c r="G24" t="str">
-        <v>Fiji</v>
+        <v>Albania</v>
       </c>
       <c r="H24" t="str">
-        <v>Blackburnbury</v>
+        <v>Nancyhaven</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" t="str">
-        <v>Smith Ltd Incubator</v>
+        <v>Kelley Ltd Incubator</v>
       </c>
       <c r="C25" t="str">
-        <v>Brooke Allen</v>
+        <v>David Baker</v>
       </c>
       <c r="D25" t="str">
-        <v>margaret59@hotmail.com</v>
+        <v>wilsonkelly@stewart-haynes.com</v>
       </c>
       <c r="E25" t="str">
-        <v>279.800.0891</v>
+        <v>(786)413-4743x078</v>
       </c>
       <c r="F25" t="str">
-        <v>Clean Energy</v>
+        <v>FinTech</v>
       </c>
       <c r="G25" t="str">
-        <v>Albania</v>
+        <v>Korea</v>
       </c>
       <c r="H25" t="str">
-        <v>Nancyhaven</v>
+        <v>Port Victoria</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" t="str">
-        <v>Kelley Ltd Incubator</v>
+        <v>Guzman PLC Incubator</v>
       </c>
       <c r="C26" t="str">
-        <v>David Baker</v>
+        <v>Donna Bailey</v>
       </c>
       <c r="D26" t="str">
-        <v>wilsonkelly@stewart-haynes.com</v>
+        <v>leahgriffin@johnson.com</v>
       </c>
       <c r="E26" t="str">
-        <v>(786)413-4743x078</v>
+        <v>(916)788-2806x26710</v>
       </c>
       <c r="F26" t="str">
-        <v>FinTech</v>
+        <v>E-commerce</v>
       </c>
       <c r="G26" t="str">
-        <v>Korea</v>
+        <v>Brunei Darussalam</v>
       </c>
       <c r="H26" t="str">
-        <v>Port Victoria</v>
+        <v>Port Lorraineport</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" t="str">
-        <v>Guzman PLC Incubator</v>
+        <v>Hudson, Dawson and Wheeler Incubator</v>
       </c>
       <c r="C27" t="str">
-        <v>Donna Bailey</v>
+        <v>Abigail Lopez</v>
       </c>
       <c r="D27" t="str">
-        <v>leahgriffin@johnson.com</v>
+        <v>wsims@hotmail.com</v>
       </c>
       <c r="E27" t="str">
-        <v>(916)788-2806x26710</v>
+        <v>693-094-5494</v>
       </c>
       <c r="F27" t="str">
-        <v>E-commerce</v>
+        <v>Biotech</v>
       </c>
       <c r="G27" t="str">
-        <v>Brunei Darussalam</v>
+        <v>Tokelau</v>
       </c>
       <c r="H27" t="str">
-        <v>Port Lorraineport</v>
+        <v>Deborahborough</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28" t="str">
-        <v>Hudson, Dawson and Wheeler Incubator</v>
+        <v>Jenkins, Boyd and Cross Incubator</v>
       </c>
       <c r="C28" t="str">
-        <v>Abigail Lopez</v>
+        <v>Barbara Cervantes MD</v>
       </c>
       <c r="D28" t="str">
-        <v>wsims@hotmail.com</v>
+        <v>michael75@gmail.com</v>
       </c>
       <c r="E28" t="str">
-        <v>693-094-5494</v>
+        <v>102.576.0492x7428</v>
       </c>
       <c r="F28" t="str">
         <v>Biotech</v>
       </c>
       <c r="G28" t="str">
-        <v>Tokelau</v>
+        <v>Papua New Guinea</v>
       </c>
       <c r="H28" t="str">
-        <v>Deborahborough</v>
+        <v>Sandraland</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B29" t="str">
-        <v>Jenkins, Boyd and Cross Incubator</v>
+        <v>Mckinney, Nelson and Blair Incubator</v>
       </c>
       <c r="C29" t="str">
-        <v>Barbara Cervantes MD</v>
+        <v>Sara White</v>
       </c>
       <c r="D29" t="str">
-        <v>michael75@gmail.com</v>
+        <v>oswanson@lewis-mullins.org</v>
       </c>
       <c r="E29" t="str">
-        <v>102.576.0492x7428</v>
+        <v>068-708-6388x2893</v>
       </c>
       <c r="F29" t="str">
-        <v>Biotech</v>
+        <v>Cybersecurity</v>
       </c>
       <c r="G29" t="str">
-        <v>Papua New Guinea</v>
+        <v>Kuwait</v>
       </c>
       <c r="H29" t="str">
-        <v>Sandraland</v>
+        <v>Savannahbury</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B30" t="str">
-        <v>Mckinney, Nelson and Blair Incubator</v>
+        <v>Chavez PLC Incubator</v>
       </c>
       <c r="C30" t="str">
-        <v>Sara White</v>
+        <v>Christian Foley</v>
       </c>
       <c r="D30" t="str">
-        <v>oswanson@lewis-mullins.org</v>
+        <v>duffystephen@gmail.com</v>
       </c>
       <c r="E30" t="str">
-        <v>068-708-6388x2893</v>
+        <v>252.175.7067x8418</v>
       </c>
       <c r="F30" t="str">
-        <v>Cybersecurity</v>
+        <v>HealthTech</v>
       </c>
       <c r="G30" t="str">
-        <v>Kuwait</v>
+        <v>Tokelau</v>
       </c>
       <c r="H30" t="str">
-        <v>Savannahbury</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31" t="str">
-        <v>Chavez PLC Incubator</v>
-      </c>
-      <c r="C31" t="str">
-        <v>Christian Foley</v>
-      </c>
-      <c r="D31" t="str">
-        <v>duffystephen@gmail.com</v>
-      </c>
-      <c r="E31" t="str">
-        <v>252.175.7067x8418</v>
-      </c>
-      <c r="F31" t="str">
-        <v>HealthTech</v>
-      </c>
-      <c r="G31" t="str">
-        <v>Tokelau</v>
-      </c>
-      <c r="H31" t="str">
         <v>West Cindy</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H31"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H30"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(incubators): align UI to investors, add view/edit modals, blue buttons, fix columns syntax
</commit_message>
<xml_diff>
--- a/backend/data/incubators.xlsx
+++ b/backend/data/incubators.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -430,761 +430,735 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="str">
-        <v>Baker, Salas and Nelson Incubator</v>
+        <v>Schaefer-Campbell Incubator</v>
       </c>
       <c r="C2" t="str">
-        <v>Laura Taylor DVM</v>
+        <v>Gene Dalton V</v>
       </c>
       <c r="D2" t="str">
-        <v>andrea11@lawrence.com</v>
+        <v>abell@gmail.com</v>
       </c>
       <c r="E2" t="str">
-        <v>+1-045-525-6450x772</v>
+        <v>522-600-9691x758</v>
       </c>
       <c r="F2" t="str">
-        <v>Blockchain</v>
+        <v>AI/ML</v>
       </c>
       <c r="G2" t="str">
-        <v>Lesotho</v>
+        <v>Serbia</v>
       </c>
       <c r="H2" t="str">
-        <v>Justinland</v>
+        <v>North Theresatown</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" t="str">
-        <v>Schaefer-Campbell Incubator</v>
+        <v>Stewart Group Incubator</v>
       </c>
       <c r="C3" t="str">
-        <v>Gene Dalton V</v>
+        <v>Courtney Downs</v>
       </c>
       <c r="D3" t="str">
-        <v>abell@gmail.com</v>
+        <v>roysmith@barber.biz</v>
       </c>
       <c r="E3" t="str">
-        <v>522-600-9691x758</v>
+        <v>291.776.4474x125</v>
       </c>
       <c r="F3" t="str">
-        <v>AI/ML</v>
+        <v>FinTech</v>
       </c>
       <c r="G3" t="str">
-        <v>Serbia</v>
+        <v>Burundi</v>
       </c>
       <c r="H3" t="str">
-        <v>North Theresatown</v>
+        <v>Brittanytown</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="str">
-        <v>Stewart Group Incubator</v>
+        <v>Fernandez-Diaz Incubator</v>
       </c>
       <c r="C4" t="str">
-        <v>Courtney Downs</v>
+        <v>David Cohen</v>
       </c>
       <c r="D4" t="str">
-        <v>roysmith@barber.biz</v>
+        <v>stephaniefoley@hotmail.com</v>
       </c>
       <c r="E4" t="str">
-        <v>291.776.4474x125</v>
+        <v>001-858-910-8567x3167</v>
       </c>
       <c r="F4" t="str">
-        <v>FinTech</v>
+        <v>AgriTech</v>
       </c>
       <c r="G4" t="str">
-        <v>Burundi</v>
+        <v>Korea</v>
       </c>
       <c r="H4" t="str">
-        <v>Brittanytown</v>
+        <v>East Stephen</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" t="str">
-        <v>Fernandez-Diaz Incubator</v>
+        <v>Ortega PLC Incubator</v>
       </c>
       <c r="C5" t="str">
-        <v>David Cohen</v>
+        <v>Allison Campbell</v>
       </c>
       <c r="D5" t="str">
-        <v>stephaniefoley@hotmail.com</v>
+        <v>cassidy84@hotmail.com</v>
       </c>
       <c r="E5" t="str">
-        <v>001-858-910-8567x3167</v>
+        <v>+1-369-183-5529</v>
       </c>
       <c r="F5" t="str">
-        <v>AgriTech</v>
+        <v>Cybersecurity</v>
       </c>
       <c r="G5" t="str">
-        <v>Korea</v>
+        <v>Azerbaijan</v>
       </c>
       <c r="H5" t="str">
-        <v>East Stephen</v>
+        <v>Davisshire</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" t="str">
-        <v>Ortega PLC Incubator</v>
+        <v>Young-Long Incubator</v>
       </c>
       <c r="C6" t="str">
-        <v>Allison Campbell</v>
+        <v>Bryan Salinas</v>
       </c>
       <c r="D6" t="str">
-        <v>cassidy84@hotmail.com</v>
+        <v>deannamason@acosta.com</v>
       </c>
       <c r="E6" t="str">
-        <v>+1-369-183-5529</v>
+        <v>907-601-2755</v>
       </c>
       <c r="F6" t="str">
-        <v>Cybersecurity</v>
+        <v>Biotech</v>
       </c>
       <c r="G6" t="str">
-        <v>Azerbaijan</v>
+        <v>Qatar</v>
       </c>
       <c r="H6" t="str">
-        <v>Davisshire</v>
+        <v>Kristenchester</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" t="str">
-        <v>Young-Long Incubator</v>
+        <v>Trujillo Ltd Incubator</v>
       </c>
       <c r="C7" t="str">
-        <v>Bryan Salinas</v>
+        <v>Joshua Serrano</v>
       </c>
       <c r="D7" t="str">
-        <v>deannamason@acosta.com</v>
+        <v>grayrobert@gmail.com</v>
       </c>
       <c r="E7" t="str">
-        <v>907-601-2755</v>
+        <v>4458470430</v>
       </c>
       <c r="F7" t="str">
-        <v>Biotech</v>
+        <v>Blockchain</v>
       </c>
       <c r="G7" t="str">
-        <v>Qatar</v>
+        <v>Sao Tome and Principe</v>
       </c>
       <c r="H7" t="str">
-        <v>Kristenchester</v>
+        <v>Kellyfort</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" t="str">
-        <v>Trujillo Ltd Incubator</v>
+        <v>Kennedy Inc Incubator</v>
       </c>
       <c r="C8" t="str">
-        <v>Joshua Serrano</v>
+        <v>Sean Wood</v>
       </c>
       <c r="D8" t="str">
-        <v>grayrobert@gmail.com</v>
+        <v>irodriguez@krueger.com</v>
       </c>
       <c r="E8" t="str">
-        <v>4458470430</v>
+        <v>282.841.0371x484</v>
       </c>
       <c r="F8" t="str">
         <v>Blockchain</v>
       </c>
       <c r="G8" t="str">
-        <v>Sao Tome and Principe</v>
+        <v>Belarus</v>
       </c>
       <c r="H8" t="str">
-        <v>Kellyfort</v>
+        <v>East Martin</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" t="str">
-        <v>Kennedy Inc Incubator</v>
+        <v>Vaughn, Davis and Robinson Incubator</v>
       </c>
       <c r="C9" t="str">
-        <v>Sean Wood</v>
+        <v>Albert Colon</v>
       </c>
       <c r="D9" t="str">
-        <v>irodriguez@krueger.com</v>
+        <v>juanguzman@yahoo.com</v>
       </c>
       <c r="E9" t="str">
-        <v>282.841.0371x484</v>
+        <v>057.692.9204x97248</v>
       </c>
       <c r="F9" t="str">
-        <v>Blockchain</v>
+        <v>FinTech</v>
       </c>
       <c r="G9" t="str">
-        <v>Belarus</v>
+        <v>Togo</v>
       </c>
       <c r="H9" t="str">
-        <v>East Martin</v>
+        <v>Carrollburgh</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" t="str">
-        <v>Vaughn, Davis and Robinson Incubator</v>
+        <v>Adams Inc Incubator</v>
       </c>
       <c r="C10" t="str">
-        <v>Albert Colon</v>
+        <v>Kenneth Houston</v>
       </c>
       <c r="D10" t="str">
-        <v>juanguzman@yahoo.com</v>
+        <v>john38@gmail.com</v>
       </c>
       <c r="E10" t="str">
-        <v>057.692.9204x97248</v>
+        <v>001-157-142-5360x4951</v>
       </c>
       <c r="F10" t="str">
-        <v>FinTech</v>
+        <v>HealthTech</v>
       </c>
       <c r="G10" t="str">
-        <v>Togo</v>
+        <v>Senegal</v>
       </c>
       <c r="H10" t="str">
-        <v>Carrollburgh</v>
+        <v>East Maryhaven</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" t="str">
-        <v>Adams Inc Incubator</v>
+        <v>Weaver LLC Incubator</v>
       </c>
       <c r="C11" t="str">
-        <v>Kenneth Houston</v>
+        <v>Robin Gonzales</v>
       </c>
       <c r="D11" t="str">
-        <v>john38@gmail.com</v>
+        <v>millerlinda@gmail.com</v>
       </c>
       <c r="E11" t="str">
-        <v>001-157-142-5360x4951</v>
+        <v>001-846-397-7006x1003</v>
       </c>
       <c r="F11" t="str">
-        <v>HealthTech</v>
+        <v>FinTech</v>
       </c>
       <c r="G11" t="str">
-        <v>Senegal</v>
+        <v>Tajikistan</v>
       </c>
       <c r="H11" t="str">
-        <v>East Maryhaven</v>
+        <v>West Ellen</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12" t="str">
-        <v>Weaver LLC Incubator</v>
+        <v>Adams, Monroe and Bell Incubator</v>
       </c>
       <c r="C12" t="str">
-        <v>Robin Gonzales</v>
+        <v>Jeffrey Maynard</v>
       </c>
       <c r="D12" t="str">
-        <v>millerlinda@gmail.com</v>
+        <v>rebeccaperry@hotmail.com</v>
       </c>
       <c r="E12" t="str">
-        <v>001-846-397-7006x1003</v>
+        <v>364.945.1421</v>
       </c>
       <c r="F12" t="str">
-        <v>FinTech</v>
+        <v>Biotech</v>
       </c>
       <c r="G12" t="str">
-        <v>Tajikistan</v>
+        <v>Faroe Islands</v>
       </c>
       <c r="H12" t="str">
-        <v>West Ellen</v>
+        <v>East Cathybury</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B13" t="str">
-        <v>Adams, Monroe and Bell Incubator</v>
+        <v>Bates, Haas and Williams Incubator</v>
       </c>
       <c r="C13" t="str">
-        <v>Jeffrey Maynard</v>
+        <v>Brian Washington</v>
       </c>
       <c r="D13" t="str">
-        <v>rebeccaperry@hotmail.com</v>
+        <v>normafarmer@fuller.com</v>
       </c>
       <c r="E13" t="str">
-        <v>364.945.1421</v>
+        <v>001-053-359-0570x9871</v>
       </c>
       <c r="F13" t="str">
-        <v>Biotech</v>
+        <v>HealthTech</v>
       </c>
       <c r="G13" t="str">
-        <v>Faroe Islands</v>
+        <v>Mozambique</v>
       </c>
       <c r="H13" t="str">
-        <v>East Cathybury</v>
+        <v>Anthonyton</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B14" t="str">
-        <v>Bates, Haas and Williams Incubator</v>
+        <v>Phillips LLC Incubator</v>
       </c>
       <c r="C14" t="str">
-        <v>Brian Washington</v>
+        <v>Brandon Wallace</v>
       </c>
       <c r="D14" t="str">
-        <v>normafarmer@fuller.com</v>
+        <v>amymanning@lewis-henry.com</v>
       </c>
       <c r="E14" t="str">
-        <v>001-053-359-0570x9871</v>
+        <v>367-518-8179x871</v>
       </c>
       <c r="F14" t="str">
-        <v>HealthTech</v>
+        <v>Blockchain</v>
       </c>
       <c r="G14" t="str">
-        <v>Mozambique</v>
+        <v>Andorra</v>
       </c>
       <c r="H14" t="str">
-        <v>Anthonyton</v>
+        <v>North Josephburgh</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B15" t="str">
-        <v>Phillips LLC Incubator</v>
+        <v>Alvarez, Thompson and Taylor Incubator</v>
       </c>
       <c r="C15" t="str">
-        <v>Brandon Wallace</v>
+        <v>Angelica Gamble</v>
       </c>
       <c r="D15" t="str">
-        <v>amymanning@lewis-henry.com</v>
+        <v>zarnold@hotmail.com</v>
       </c>
       <c r="E15" t="str">
-        <v>367-518-8179x871</v>
+        <v>625.796.1725x68758</v>
       </c>
       <c r="F15" t="str">
-        <v>Blockchain</v>
+        <v>AI/ML</v>
       </c>
       <c r="G15" t="str">
-        <v>Andorra</v>
+        <v>Norway</v>
       </c>
       <c r="H15" t="str">
-        <v>North Josephburgh</v>
+        <v>South Shane</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B16" t="str">
-        <v>Alvarez, Thompson and Taylor Incubator</v>
+        <v>Hall-Page Incubator</v>
       </c>
       <c r="C16" t="str">
-        <v>Angelica Gamble</v>
+        <v>Aaron Brown</v>
       </c>
       <c r="D16" t="str">
-        <v>zarnold@hotmail.com</v>
+        <v>gkirby@hotmail.com</v>
       </c>
       <c r="E16" t="str">
-        <v>625.796.1725x68758</v>
+        <v>001-542-949-4976x95178</v>
       </c>
       <c r="F16" t="str">
-        <v>AI/ML</v>
+        <v>Clean Energy</v>
       </c>
       <c r="G16" t="str">
-        <v>Norway</v>
+        <v>Uganda</v>
       </c>
       <c r="H16" t="str">
-        <v>South Shane</v>
+        <v>Shorthaven</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B17" t="str">
-        <v>Hall-Page Incubator</v>
+        <v>Deleon-Holden Incubator</v>
       </c>
       <c r="C17" t="str">
-        <v>Aaron Brown</v>
+        <v>Phillip Hull</v>
       </c>
       <c r="D17" t="str">
-        <v>gkirby@hotmail.com</v>
+        <v>msmith@swanson-andrews.com</v>
       </c>
       <c r="E17" t="str">
-        <v>001-542-949-4976x95178</v>
+        <v>001-236-186-3545x70205</v>
       </c>
       <c r="F17" t="str">
-        <v>Clean Energy</v>
+        <v>Blockchain</v>
       </c>
       <c r="G17" t="str">
-        <v>Uganda</v>
+        <v>Equatorial Guinea</v>
       </c>
       <c r="H17" t="str">
-        <v>Shorthaven</v>
+        <v>Rachelfurt</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B18" t="str">
-        <v>Deleon-Holden Incubator</v>
+        <v>Merritt, Anderson and Cross Incubator</v>
       </c>
       <c r="C18" t="str">
-        <v>Phillip Hull</v>
+        <v>Brent Thomas</v>
       </c>
       <c r="D18" t="str">
-        <v>msmith@swanson-andrews.com</v>
+        <v>donovanbailey@smith-erickson.com</v>
       </c>
       <c r="E18" t="str">
-        <v>001-236-186-3545x70205</v>
+        <v>(044)565-4201</v>
       </c>
       <c r="F18" t="str">
-        <v>Blockchain</v>
+        <v>AI/ML</v>
       </c>
       <c r="G18" t="str">
-        <v>Equatorial Guinea</v>
+        <v>Myanmar</v>
       </c>
       <c r="H18" t="str">
-        <v>Rachelfurt</v>
+        <v>West Keith</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B19" t="str">
-        <v>Merritt, Anderson and Cross Incubator</v>
+        <v>Stone-Salazar Incubator</v>
       </c>
       <c r="C19" t="str">
-        <v>Brent Thomas</v>
+        <v>Edward Hunter</v>
       </c>
       <c r="D19" t="str">
-        <v>donovanbailey@smith-erickson.com</v>
+        <v>andrea60@gmail.com</v>
       </c>
       <c r="E19" t="str">
-        <v>(044)565-4201</v>
+        <v>211.655.2758x6849</v>
       </c>
       <c r="F19" t="str">
-        <v>AI/ML</v>
+        <v>EdTech</v>
       </c>
       <c r="G19" t="str">
-        <v>Myanmar</v>
+        <v>Iran</v>
       </c>
       <c r="H19" t="str">
-        <v>West Keith</v>
+        <v>Weavertown</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B20" t="str">
-        <v>Stone-Salazar Incubator</v>
+        <v>Kaufman PLC Incubator</v>
       </c>
       <c r="C20" t="str">
-        <v>Edward Hunter</v>
+        <v>Tasha Hanson</v>
       </c>
       <c r="D20" t="str">
-        <v>andrea60@gmail.com</v>
+        <v>anitamorrison@hotmail.com</v>
       </c>
       <c r="E20" t="str">
-        <v>211.655.2758x6849</v>
+        <v>2522613276</v>
       </c>
       <c r="F20" t="str">
-        <v>EdTech</v>
+        <v>Blockchain</v>
       </c>
       <c r="G20" t="str">
-        <v>Iran</v>
+        <v>Algeria</v>
       </c>
       <c r="H20" t="str">
-        <v>Weavertown</v>
+        <v>Hensleychester</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B21" t="str">
-        <v>Kaufman PLC Incubator</v>
+        <v>Bruce-James Incubator</v>
       </c>
       <c r="C21" t="str">
-        <v>Tasha Hanson</v>
+        <v>Suzanne Matthews</v>
       </c>
       <c r="D21" t="str">
-        <v>anitamorrison@hotmail.com</v>
+        <v>hchandler@gmail.com</v>
       </c>
       <c r="E21" t="str">
-        <v>2522613276</v>
+        <v>+1-010-437-9859x119</v>
       </c>
       <c r="F21" t="str">
-        <v>Blockchain</v>
+        <v>HealthTech</v>
       </c>
       <c r="G21" t="str">
-        <v>Algeria</v>
+        <v>Aruba</v>
       </c>
       <c r="H21" t="str">
-        <v>Hensleychester</v>
+        <v>Welchchester</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B22" t="str">
-        <v>Bruce-James Incubator</v>
+        <v>Brown, Miller and Taylor Incubator</v>
       </c>
       <c r="C22" t="str">
-        <v>Suzanne Matthews</v>
+        <v>Martin Vazquez</v>
       </c>
       <c r="D22" t="str">
-        <v>hchandler@gmail.com</v>
+        <v>kwilson@hill-munoz.com</v>
       </c>
       <c r="E22" t="str">
-        <v>+1-010-437-9859x119</v>
+        <v>(397)708-5273x153</v>
       </c>
       <c r="F22" t="str">
         <v>HealthTech</v>
       </c>
       <c r="G22" t="str">
-        <v>Aruba</v>
+        <v>Fiji</v>
       </c>
       <c r="H22" t="str">
-        <v>Welchchester</v>
+        <v>Blackburnbury</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B23" t="str">
-        <v>Brown, Miller and Taylor Incubator</v>
+        <v>Smith Ltd Incubator</v>
       </c>
       <c r="C23" t="str">
-        <v>Martin Vazquez</v>
+        <v>Brooke Allen</v>
       </c>
       <c r="D23" t="str">
-        <v>kwilson@hill-munoz.com</v>
+        <v>margaret59@hotmail.com</v>
       </c>
       <c r="E23" t="str">
-        <v>(397)708-5273x153</v>
+        <v>279.800.0891</v>
       </c>
       <c r="F23" t="str">
-        <v>HealthTech</v>
+        <v>Clean Energy</v>
       </c>
       <c r="G23" t="str">
-        <v>Fiji</v>
+        <v>Albania</v>
       </c>
       <c r="H23" t="str">
-        <v>Blackburnbury</v>
+        <v>Nancyhaven</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B24" t="str">
-        <v>Smith Ltd Incubator</v>
+        <v>Kelley Ltd Incubator</v>
       </c>
       <c r="C24" t="str">
-        <v>Brooke Allen</v>
+        <v>David Baker</v>
       </c>
       <c r="D24" t="str">
-        <v>margaret59@hotmail.com</v>
+        <v>wilsonkelly@stewart-haynes.com</v>
       </c>
       <c r="E24" t="str">
-        <v>279.800.0891</v>
+        <v>(786)413-4743x078</v>
       </c>
       <c r="F24" t="str">
-        <v>Clean Energy</v>
+        <v>FinTech</v>
       </c>
       <c r="G24" t="str">
-        <v>Albania</v>
+        <v>Korea</v>
       </c>
       <c r="H24" t="str">
-        <v>Nancyhaven</v>
+        <v>Port Victoria</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B25" t="str">
-        <v>Kelley Ltd Incubator</v>
+        <v>Guzman PLC Incubator</v>
       </c>
       <c r="C25" t="str">
-        <v>David Baker</v>
+        <v>Donna Bailey</v>
       </c>
       <c r="D25" t="str">
-        <v>wilsonkelly@stewart-haynes.com</v>
+        <v>leahgriffin@johnson.com</v>
       </c>
       <c r="E25" t="str">
-        <v>(786)413-4743x078</v>
+        <v>(916)788-2806x26710</v>
       </c>
       <c r="F25" t="str">
-        <v>FinTech</v>
+        <v>E-commerce</v>
       </c>
       <c r="G25" t="str">
-        <v>Korea</v>
+        <v>Brunei Darussalam</v>
       </c>
       <c r="H25" t="str">
-        <v>Port Victoria</v>
+        <v>Port Lorraineport</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B26" t="str">
-        <v>Guzman PLC Incubator</v>
+        <v>Hudson, Dawson and Wheeler Incubator</v>
       </c>
       <c r="C26" t="str">
-        <v>Donna Bailey</v>
+        <v>Abigail Lopez</v>
       </c>
       <c r="D26" t="str">
-        <v>leahgriffin@johnson.com</v>
+        <v>wsims@hotmail.com</v>
       </c>
       <c r="E26" t="str">
-        <v>(916)788-2806x26710</v>
+        <v>693-094-5494</v>
       </c>
       <c r="F26" t="str">
-        <v>E-commerce</v>
+        <v>Biotech</v>
       </c>
       <c r="G26" t="str">
-        <v>Brunei Darussalam</v>
+        <v>Tokelau</v>
       </c>
       <c r="H26" t="str">
-        <v>Port Lorraineport</v>
+        <v>Deborahborough</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B27" t="str">
-        <v>Hudson, Dawson and Wheeler Incubator</v>
+        <v>Jenkins, Boyd and Cross Incubator</v>
       </c>
       <c r="C27" t="str">
-        <v>Abigail Lopez</v>
+        <v>Barbara Cervantes MD</v>
       </c>
       <c r="D27" t="str">
-        <v>wsims@hotmail.com</v>
+        <v>michael75@gmail.com</v>
       </c>
       <c r="E27" t="str">
-        <v>693-094-5494</v>
+        <v>102.576.0492x7428</v>
       </c>
       <c r="F27" t="str">
         <v>Biotech</v>
       </c>
       <c r="G27" t="str">
-        <v>Tokelau</v>
+        <v>Papua New Guinea</v>
       </c>
       <c r="H27" t="str">
-        <v>Deborahborough</v>
+        <v>Sandraland</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B28" t="str">
-        <v>Jenkins, Boyd and Cross Incubator</v>
+        <v>Mckinney, Nelson and Blair Incubator</v>
       </c>
       <c r="C28" t="str">
-        <v>Barbara Cervantes MD</v>
+        <v>Sara White</v>
       </c>
       <c r="D28" t="str">
-        <v>michael75@gmail.com</v>
+        <v>oswanson@lewis-mullins.org</v>
       </c>
       <c r="E28" t="str">
-        <v>102.576.0492x7428</v>
+        <v>068-708-6388x2893</v>
       </c>
       <c r="F28" t="str">
-        <v>Biotech</v>
+        <v>Cybersecurity</v>
       </c>
       <c r="G28" t="str">
-        <v>Papua New Guinea</v>
+        <v>Kuwait</v>
       </c>
       <c r="H28" t="str">
-        <v>Sandraland</v>
+        <v>Savannahbury</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B29" t="str">
-        <v>Mckinney, Nelson and Blair Incubator</v>
+        <v>Chavez PLC Incubator</v>
       </c>
       <c r="C29" t="str">
-        <v>Sara White</v>
+        <v>Christian Foley</v>
       </c>
       <c r="D29" t="str">
-        <v>oswanson@lewis-mullins.org</v>
+        <v>duffystephen@gmail.com</v>
       </c>
       <c r="E29" t="str">
-        <v>068-708-6388x2893</v>
+        <v>252.175.7067x8418</v>
       </c>
       <c r="F29" t="str">
-        <v>Cybersecurity</v>
+        <v>HealthTech</v>
       </c>
       <c r="G29" t="str">
-        <v>Kuwait</v>
+        <v>Tokelau</v>
       </c>
       <c r="H29" t="str">
-        <v>Savannahbury</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30">
-        <v>30</v>
-      </c>
-      <c r="B30" t="str">
-        <v>Chavez PLC Incubator</v>
-      </c>
-      <c r="C30" t="str">
-        <v>Christian Foley</v>
-      </c>
-      <c r="D30" t="str">
-        <v>duffystephen@gmail.com</v>
-      </c>
-      <c r="E30" t="str">
-        <v>252.175.7067x8418</v>
-      </c>
-      <c r="F30" t="str">
-        <v>HealthTech</v>
-      </c>
-      <c r="G30" t="str">
-        <v>Tokelau</v>
-      </c>
-      <c r="H30" t="str">
         <v>West Cindy</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H30"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H29"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix TypeScript errors and Vercel deployment issues - Updated Node.js version to 18.x for Vercel compatibility - Fixed missing DEFAULT_INVESTOR_TEMPLATE constant - Added proper TypeScript type annotations - Fixed API response type casting - Resolved JSX structure issues - Added .vercelignore for backend - Updated README with Vercel deployment instructions
</commit_message>
<xml_diff>
--- a/backend/data/incubators.xlsx
+++ b/backend/data/incubators.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:S33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -427,6 +427,39 @@
       <c r="H1" t="str">
         <v>stateCity</v>
       </c>
+      <c r="I1" t="str">
+        <v>name</v>
+      </c>
+      <c r="J1" t="str">
+        <v>location</v>
+      </c>
+      <c r="K1" t="str">
+        <v>website</v>
+      </c>
+      <c r="L1" t="str">
+        <v>email</v>
+      </c>
+      <c r="M1" t="str">
+        <v>phone</v>
+      </c>
+      <c r="N1" t="str">
+        <v>focus_sectors</v>
+      </c>
+      <c r="O1" t="str">
+        <v>program_duration</v>
+      </c>
+      <c r="P1" t="str">
+        <v>equity_taken</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>funding_amount</v>
+      </c>
+      <c r="R1" t="str">
+        <v>application_deadline</v>
+      </c>
+      <c r="S1" t="str">
+        <v>description</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2">
@@ -1156,9 +1189,149 @@
         <v>West Cindy</v>
       </c>
     </row>
+    <row r="30">
+      <c r="I30" t="str">
+        <v>zdvxfb</v>
+      </c>
+      <c r="J30" t="str">
+        <v/>
+      </c>
+      <c r="K30" t="str">
+        <v/>
+      </c>
+      <c r="L30" t="str">
+        <v>priyanshu@gmail.com</v>
+      </c>
+      <c r="M30" t="str">
+        <v>8103700333</v>
+      </c>
+      <c r="N30" t="str">
+        <v>kk</v>
+      </c>
+      <c r="O30" t="str">
+        <v/>
+      </c>
+      <c r="P30" t="str">
+        <v/>
+      </c>
+      <c r="Q30" t="str">
+        <v/>
+      </c>
+      <c r="R30" t="str">
+        <v/>
+      </c>
+      <c r="S30" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="31">
+      <c r="I31" t="str">
+        <v>pari</v>
+      </c>
+      <c r="J31" t="str">
+        <v/>
+      </c>
+      <c r="K31" t="str">
+        <v/>
+      </c>
+      <c r="L31" t="str">
+        <v>priyanshu@gmail.com</v>
+      </c>
+      <c r="M31" t="str">
+        <v>8103700333</v>
+      </c>
+      <c r="N31" t="str">
+        <v>kk</v>
+      </c>
+      <c r="O31" t="str">
+        <v/>
+      </c>
+      <c r="P31" t="str">
+        <v/>
+      </c>
+      <c r="Q31" t="str">
+        <v/>
+      </c>
+      <c r="R31" t="str">
+        <v/>
+      </c>
+      <c r="S31" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="32">
+      <c r="I32" t="str">
+        <v>pari</v>
+      </c>
+      <c r="J32" t="str">
+        <v/>
+      </c>
+      <c r="K32" t="str">
+        <v/>
+      </c>
+      <c r="L32" t="str">
+        <v>priyanshu@gmail.com</v>
+      </c>
+      <c r="M32" t="str">
+        <v>8103700333</v>
+      </c>
+      <c r="N32" t="str">
+        <v>kk</v>
+      </c>
+      <c r="O32" t="str">
+        <v/>
+      </c>
+      <c r="P32" t="str">
+        <v/>
+      </c>
+      <c r="Q32" t="str">
+        <v/>
+      </c>
+      <c r="R32" t="str">
+        <v/>
+      </c>
+      <c r="S32" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="33">
+      <c r="I33" t="str">
+        <v>pari</v>
+      </c>
+      <c r="J33" t="str">
+        <v/>
+      </c>
+      <c r="K33" t="str">
+        <v/>
+      </c>
+      <c r="L33" t="str">
+        <v>priyanshu@gmail.com</v>
+      </c>
+      <c r="M33" t="str">
+        <v>8103700333</v>
+      </c>
+      <c r="N33" t="str">
+        <v>kk</v>
+      </c>
+      <c r="O33" t="str">
+        <v/>
+      </c>
+      <c r="P33" t="str">
+        <v/>
+      </c>
+      <c r="Q33" t="str">
+        <v/>
+      </c>
+      <c r="R33" t="str">
+        <v/>
+      </c>
+      <c r="S33" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H29"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:S33"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>